<commit_message>
added data to csv and created scatter plot
</commit_message>
<xml_diff>
--- a/Demographic_data.xlsx
+++ b/Demographic_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amykerdolff/Documents/Documents/Visual Studio Code/Plotting practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4664CA5-40E8-8848-BDC4-90F72ABD5AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C82115A-72AE-F248-AD5D-437A48800566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" xr2:uid="{6ED43592-84A2-E748-97DD-C2A9A8C8DCD7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t>Customer ID</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Monthly Household Income</t>
+  </si>
+  <si>
+    <t>Household Size</t>
   </si>
 </sst>
 </file>
@@ -516,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E5308E-CF5C-7E4A-B88A-70D4AC053766}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -530,7 +533,7 @@
     <col min="8" max="8" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -555,8 +558,11 @@
       <c r="H1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -581,8 +587,11 @@
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -607,8 +616,11 @@
       <c r="H3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -631,10 +643,13 @@
         <v>37</v>
       </c>
       <c r="H4">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2000</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -659,8 +674,11 @@
       <c r="H5">
         <v>1200</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -685,8 +703,11 @@
       <c r="H6">
         <v>3000</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -709,10 +730,13 @@
         <v>38</v>
       </c>
       <c r="H7">
-        <v>3750</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -737,8 +761,11 @@
       <c r="H8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -761,10 +788,13 @@
         <v>37</v>
       </c>
       <c r="H9">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -787,10 +817,13 @@
         <v>37</v>
       </c>
       <c r="H10">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -814,6 +847,9 @@
       </c>
       <c r="H11">
         <v>500</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>